<commit_message>
completed have some giberrish as well
</commit_message>
<xml_diff>
--- a/webscraping/email-and-phone-scraper-master/Florida.xlsx
+++ b/webscraping/email-and-phone-scraper-master/Florida.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naman/Desktop/WebScrapeWebsitesEmails/final_locations_to_scrap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naman/Desktop/WebScrapeWebsitesEmails/webscraping/email-and-phone-scraper-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D43114-78CB-7848-B9C4-8A58757AE4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C61D05-6A74-0B48-98D5-97239A69FA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45860" yWindow="500" windowWidth="22940" windowHeight="26580" xr2:uid="{52A1A797-E0A8-1C45-91AE-CCC580E4E5FE}"/>
+    <workbookView xWindow="3680" yWindow="500" windowWidth="34400" windowHeight="26580" xr2:uid="{52A1A797-E0A8-1C45-91AE-CCC580E4E5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -113,9 +113,6 @@
     <t>5501 Northwest 36th Ave.</t>
   </si>
   <si>
-    <t>2254 Trade Center Way</t>
-  </si>
-  <si>
     <t>GDI Technology Inc./Secure Destruct Services Corporation</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>1678 Independence Blvd, Suite B</t>
   </si>
   <si>
-    <t>3661 S. Pine Avenue</t>
-  </si>
-  <si>
     <t>RSR Partners, LLC dba Regency Technologies</t>
   </si>
   <si>
@@ -197,79 +191,73 @@
     <t>Suite 303 and 305, 4400 118th Ave. North</t>
   </si>
   <si>
-    <t>auditmacstech.com</t>
-  </si>
-  <si>
-    <t>cleanearthinc.com</t>
-  </si>
-  <si>
-    <t>digitaltechmia.com</t>
-  </si>
-  <si>
-    <t>http://www.reaganwireless.com/</t>
-  </si>
-  <si>
     <t>https://www.earlyupgrade.com</t>
   </si>
   <si>
     <t>https://www.q1w.com/</t>
   </si>
   <si>
-    <t>www.a1assets.com</t>
-  </si>
-  <si>
     <t>WWW.CENTURYPCINC.COM</t>
   </si>
   <si>
-    <t>www.citizoneusa.com</t>
-  </si>
-  <si>
-    <t>www.ercrecycling.com</t>
-  </si>
-  <si>
-    <t>www.exittechnologies.com</t>
-  </si>
-  <si>
-    <t>www.gditechnology.com</t>
-  </si>
-  <si>
-    <t>www.gonextleveltech.com</t>
-  </si>
-  <si>
-    <t>www.hubx.com</t>
-  </si>
-  <si>
-    <t>www.intechar.com</t>
-  </si>
-  <si>
-    <t>www.RAEIT.com</t>
-  </si>
-  <si>
-    <t>www.regencytechnologies.com</t>
-  </si>
-  <si>
-    <t>www.sbnetworkit.com</t>
-  </si>
-  <si>
-    <t>www.streamrecycling.com</t>
-  </si>
-  <si>
-    <t>www.techassetrecovery.com</t>
-  </si>
-  <si>
-    <t>www.telecomnetworksupply.com</t>
-  </si>
-  <si>
-    <t>www.toppsolutions.com</t>
-  </si>
-  <si>
-    <t>www.unicor.gov</t>
-  </si>
-  <si>
     <t>www.westworldtelecom.com</t>
   </si>
   <si>
     <t>www.yijep.com</t>
+  </si>
+  <si>
+    <t>https://auditmacstech.com/</t>
+  </si>
+  <si>
+    <t>https://www.cleanearthinc.com/</t>
+  </si>
+  <si>
+    <t>https://www.digitaltechmia.com/</t>
+  </si>
+  <si>
+    <t>https://www.reaganwireless.com/</t>
+  </si>
+  <si>
+    <t>https://a1assets.com/site/</t>
+  </si>
+  <si>
+    <t>https://www.citizoneusa.com/</t>
+  </si>
+  <si>
+    <t>https://www.ercrecycling.com/</t>
+  </si>
+  <si>
+    <t>https://www.gditechnology.com/</t>
+  </si>
+  <si>
+    <t>https://gonextleveltech.com/</t>
+  </si>
+  <si>
+    <t>https://www.hubx.com/</t>
+  </si>
+  <si>
+    <t>https://intechar.com/</t>
+  </si>
+  <si>
+    <t>https://regencytechnologies.com/</t>
+  </si>
+  <si>
+    <t>https://www.sbnetworkit.com/</t>
+  </si>
+  <si>
+    <t>https://www.streamrecycling.com/</t>
+  </si>
+  <si>
+    <t>https://techassetrecovery.com/</t>
+  </si>
+  <si>
+    <t>https://telecomnetworksupply.com/</t>
+  </si>
+  <si>
+    <t>https://www.toppsolutions.com/</t>
+  </si>
+  <si>
+    <t>https://www.unicor.gov/</t>
   </si>
 </sst>
 </file>
@@ -648,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855C4575-822D-684E-8920-2D8CDF16DFDE}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -698,7 +686,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -709,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -720,7 +708,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -731,7 +719,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -742,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -753,7 +741,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -764,7 +752,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -790,9 +778,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>63</v>
@@ -800,21 +790,21 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>64</v>
@@ -822,10 +812,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>65</v>
@@ -833,10 +823,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>66</v>
@@ -844,19 +834,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>68</v>
@@ -864,10 +856,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>69</v>
@@ -875,10 +867,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>70</v>
@@ -886,10 +878,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>71</v>
@@ -897,10 +889,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>72</v>
@@ -908,10 +900,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>73</v>
@@ -919,76 +911,35 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://auditmacstech.com/" xr:uid="{6D58AB85-2158-3D49-8ECA-74D2919BC07B}"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://cleanearthinc.com/" xr:uid="{7749A8D1-FEAC-324D-B36E-8478BF4C49F6}"/>
-    <hyperlink ref="C4" r:id="rId3" display="http://digitaltechmia.com/" xr:uid="{B875FCE4-0795-CA41-9FF9-4BDD2FC514C5}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{EBB47F4B-2F9E-B845-AB2D-3545D39E83DA}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://www.earlyupgrade.com/" xr:uid="{F343DEC8-6C8E-7F42-BD58-976CC505132D}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{42D4975D-1F31-B446-8F1F-BC40A1696DE0}"/>
-    <hyperlink ref="C8" r:id="rId7" display="http://www.a1assets.com/" xr:uid="{63B86A85-D0D0-1647-A82B-790084810938}"/>
-    <hyperlink ref="C9" r:id="rId8" display="http://www.centurypcinc.com/" xr:uid="{C9B9E30C-6E2D-E146-972A-626B471FAD4C}"/>
-    <hyperlink ref="C10" r:id="rId9" display="http://www.citizoneusa.com/" xr:uid="{98E45EB5-D815-EB4E-A83C-FCC189A931DC}"/>
-    <hyperlink ref="C11" r:id="rId10" display="http://www.ercrecycling.com/" xr:uid="{F44468B4-C054-8844-9098-27EF94D36EF4}"/>
-    <hyperlink ref="C12" r:id="rId11" display="http://www.exittechnologies.com/" xr:uid="{A62F0799-A404-E548-A894-9C9F4470E856}"/>
-    <hyperlink ref="C13" r:id="rId12" display="http://www.gditechnology.com/" xr:uid="{03FA6B23-4F58-A546-B807-297A5EEEA741}"/>
-    <hyperlink ref="C14" r:id="rId13" display="http://www.gditechnology.com/" xr:uid="{C1B542E4-ABCD-2649-B17B-2BB0F4E5F535}"/>
-    <hyperlink ref="C15" r:id="rId14" display="http://www.gonextleveltech.com/" xr:uid="{88422086-963D-8B43-B2E4-C4AFC1E3E9EB}"/>
-    <hyperlink ref="C16" r:id="rId15" display="http://www.hubx.com/" xr:uid="{EA573E19-0AA6-CE4D-950E-9B308A399F4D}"/>
-    <hyperlink ref="C17" r:id="rId16" display="http://www.intechar.com/" xr:uid="{57F78885-6C3A-6042-9B97-041A153AAA1F}"/>
-    <hyperlink ref="C18" r:id="rId17" display="http://www.raeit.com/" xr:uid="{D1E933AE-D867-4E46-9E9C-70F5295633A6}"/>
-    <hyperlink ref="C19" r:id="rId18" display="http://www.regencytechnologies.com/" xr:uid="{E2101B64-3D90-9B40-952B-935B1A639017}"/>
-    <hyperlink ref="C20" r:id="rId19" display="http://www.sbnetworkit.com/" xr:uid="{44C7643B-6F66-1C41-89A2-90883B304092}"/>
-    <hyperlink ref="C21" r:id="rId20" display="http://www.streamrecycling.com/" xr:uid="{D95B205C-C872-2648-8041-0C864400271E}"/>
-    <hyperlink ref="C22" r:id="rId21" display="http://www.techassetrecovery.com/" xr:uid="{3683283D-414A-2A4F-BD47-0348CF6E28A8}"/>
-    <hyperlink ref="C23" r:id="rId22" display="http://www.telecomnetworksupply.com/" xr:uid="{7A5A0D0C-6553-7744-903B-7F79752F2B59}"/>
-    <hyperlink ref="C24" r:id="rId23" display="http://www.toppsolutions.com/" xr:uid="{5FABD8CE-D00E-8249-8AAE-3A19148C8D05}"/>
-    <hyperlink ref="C25" r:id="rId24" display="http://www.unicor.gov/" xr:uid="{ED0970C6-7468-6A45-937C-E34EB52AAA5B}"/>
-    <hyperlink ref="C26" r:id="rId25" display="http://www.westworldtelecom.com/" xr:uid="{4C23897C-2810-8A4C-8D3B-7524C8A9E20C}"/>
-    <hyperlink ref="C27" r:id="rId26" display="http://www.yijep.com/" xr:uid="{6D98EF43-E711-CD46-9FE2-5EA296009568}"/>
+    <hyperlink ref="C6" r:id="rId1" display="https://www.earlyupgrade.com/" xr:uid="{F343DEC8-6C8E-7F42-BD58-976CC505132D}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{42D4975D-1F31-B446-8F1F-BC40A1696DE0}"/>
+    <hyperlink ref="C9" r:id="rId3" display="http://www.centurypcinc.com/" xr:uid="{C9B9E30C-6E2D-E146-972A-626B471FAD4C}"/>
+    <hyperlink ref="C13" r:id="rId4" xr:uid="{C1B542E4-ABCD-2649-B17B-2BB0F4E5F535}"/>
+    <hyperlink ref="C15" r:id="rId5" xr:uid="{EA573E19-0AA6-CE4D-950E-9B308A399F4D}"/>
+    <hyperlink ref="C24" r:id="rId6" display="http://www.westworldtelecom.com/" xr:uid="{4C23897C-2810-8A4C-8D3B-7524C8A9E20C}"/>
+    <hyperlink ref="C25" r:id="rId7" display="http://www.yijep.com/" xr:uid="{6D98EF43-E711-CD46-9FE2-5EA296009568}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>